<commit_message>
chart property adding to the worksheet...
</commit_message>
<xml_diff>
--- a/tests/demo.xlsx
+++ b/tests/demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t xml:space="preserve">Age</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t xml:space="preserve">Weight / Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
   </si>
 </sst>
 </file>
@@ -130,7 +142,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -158,6 +170,21 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -256,7 +283,394 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>TITLE!!!</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>test</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$23:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="91509291"/>
+        <c:axId val="12235995"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="91509291"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>TITLE_x</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="12235995"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="12235995"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>TITLE_y</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91509291"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -270,9 +684,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>324720</xdr:colOff>
+      <xdr:colOff>324360</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -282,7 +696,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1">
           <a:off x="2905200" y="830520"/>
-          <a:ext cx="981720" cy="29160"/>
+          <a:ext cx="981360" cy="28800"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -332,9 +746,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>600480</xdr:colOff>
+      <xdr:colOff>600120</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -344,7 +758,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3874680" y="556200"/>
-          <a:ext cx="1050120" cy="653760"/>
+          <a:ext cx="1049760" cy="653400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -452,15 +866,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>59400</xdr:colOff>
+      <xdr:colOff>58680</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>355320</xdr:colOff>
+      <xdr:colOff>354240</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -469,8 +883,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="2859480" y="2277000"/>
-          <a:ext cx="295920" cy="272880"/>
+          <a:off x="2858760" y="2276280"/>
+          <a:ext cx="295560" cy="272520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -520,9 +934,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>371880</xdr:colOff>
+      <xdr:colOff>371520</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -532,7 +946,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2883960" y="2575440"/>
-          <a:ext cx="1050120" cy="653760"/>
+          <a:ext cx="1049760" cy="653400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -646,9 +1060,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>317520</xdr:colOff>
+      <xdr:colOff>317160</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -658,7 +1072,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="8521560" y="1149120"/>
-          <a:ext cx="692280" cy="356760"/>
+          <a:ext cx="691920" cy="356400"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -708,9 +1122,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>364320</xdr:colOff>
+      <xdr:colOff>363960</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -720,7 +1134,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8598960" y="1562040"/>
-          <a:ext cx="1423440" cy="653760"/>
+          <a:ext cx="1423080" cy="653400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -825,6 +1239,36 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>501840</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>119160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>670320</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="2282760" y="3411000"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -833,10 +1277,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K29" activeCellId="0" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1100,6 +1544,39 @@
       <c r="F12" s="4" t="n">
         <f aca="false">F11/F10</f>
         <v>1.83333333333333</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1125,13 +1602,13 @@
   </sheetPr>
   <dimension ref="C13:J36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
completed and updated dependencies
</commit_message>
<xml_diff>
--- a/tests/demo.xlsx
+++ b/tests/demo.xlsx
@@ -153,9 +153,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="0.00000;[RED]\-0.00000"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -537,6 +539,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -561,12 +567,8 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -749,7 +751,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -871,11 +873,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="23818541"/>
-        <c:axId val="91278636"/>
+        <c:axId val="65390968"/>
+        <c:axId val="67308049"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="23818541"/>
+        <c:axId val="65390968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,14 +942,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91278636"/>
+        <c:crossAx val="67308049"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91278636"/>
+        <c:axId val="67308049"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,7 +1023,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23818541"/>
+        <c:crossAx val="65390968"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1073,15 +1075,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>103320</xdr:colOff>
+      <xdr:colOff>102600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>99720</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>320400</xdr:colOff>
+      <xdr:colOff>318600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1090,8 +1092,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2905920" y="823320"/>
-          <a:ext cx="979200" cy="26640"/>
+          <a:off x="2905200" y="823680"/>
+          <a:ext cx="978120" cy="25920"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1141,9 +1143,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>598320</xdr:colOff>
+      <xdr:colOff>597600</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1153,7 +1155,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3877560" y="556200"/>
-          <a:ext cx="1047600" cy="636480"/>
+          <a:ext cx="1046880" cy="636120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1237,15 +1239,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>487080</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:colOff>192600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>182160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>781200</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:colOff>486000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1254,8 +1256,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="2269440" y="1717200"/>
-          <a:ext cx="294120" cy="270360"/>
+          <a:off x="1974960" y="1446840"/>
+          <a:ext cx="293400" cy="269640"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1299,15 +1301,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>84240</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>369720</xdr:colOff>
+      <xdr:colOff>369000</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>117720</xdr:rowOff>
+      <xdr:rowOff>117000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1316,8 +1318,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2886840" y="2553120"/>
-          <a:ext cx="1047600" cy="627840"/>
+          <a:off x="2887200" y="2553480"/>
+          <a:ext cx="1046520" cy="626760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1400,16 +1402,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>528840</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600120</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>456840</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>527400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>55080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1418,8 +1420,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="7141680" y="422280"/>
-          <a:ext cx="689760" cy="354240"/>
+          <a:off x="6450840" y="66960"/>
+          <a:ext cx="689400" cy="353880"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1465,13 +1467,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>465120</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>99720</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>362160</xdr:colOff>
+      <xdr:colOff>361800</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1480,8 +1482,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8601840" y="1547280"/>
-          <a:ext cx="1420920" cy="651240"/>
+          <a:off x="8601840" y="1547640"/>
+          <a:ext cx="1420560" cy="650520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1567,13 +1569,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>501840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>668160</xdr:colOff>
+      <xdr:colOff>667800</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1581,8 +1583,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2284200" y="3358080"/>
-        <a:ext cx="5758560" cy="3245040"/>
+        <a:off x="2284200" y="3724920"/>
+        <a:ext cx="5758200" cy="3243960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1603,7 +1605,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O21" activeCellId="0" sqref="O21:Q25"/>
+      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1611,7 +1613,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="9.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,7 +2016,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="42.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K18" s="0" t="n">
         <v>17</v>
       </c>
@@ -2024,11 +2028,11 @@
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
-      <c r="N18" s="13" t="n">
-        <f aca="false">$N$11</f>
-        <v>123456789</v>
-      </c>
-      <c r="O18" s="18" t="n">
+      <c r="N18" s="18" t="n">
+        <f aca="false">-SQRT($N$11)</f>
+        <v>-11111.1110605556</v>
+      </c>
+      <c r="O18" s="19" t="n">
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
@@ -2036,7 +2040,7 @@
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
-      <c r="Q18" s="19" t="n">
+      <c r="Q18" s="20" t="n">
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
@@ -2045,7 +2049,7 @@
       <c r="K19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="L19" s="20" t="n">
+      <c r="L19" s="21" t="n">
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
@@ -2057,7 +2061,7 @@
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
-      <c r="O19" s="21" t="n">
+      <c r="O19" s="22" t="n">
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
@@ -2065,7 +2069,7 @@
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
-      <c r="Q19" s="22" t="n">
+      <c r="Q19" s="23" t="n">
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
@@ -2074,7 +2078,7 @@
       <c r="K20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="L20" s="23" t="n">
+      <c r="L20" s="24" t="n">
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
@@ -2082,15 +2086,15 @@
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
-      <c r="N20" s="13" t="n">
-        <f aca="false">$N$11</f>
-        <v>123456789</v>
-      </c>
-      <c r="O20" s="24" t="n">
-        <f aca="false">$N$11</f>
-        <v>123456789</v>
-      </c>
-      <c r="P20" s="13" t="n">
+      <c r="N20" s="25" t="n">
+        <f aca="false">$N$11/-42.42</f>
+        <v>-2910343.91796322</v>
+      </c>
+      <c r="O20" s="25" t="n">
+        <f aca="false">$N$11</f>
+        <v>123456789</v>
+      </c>
+      <c r="P20" s="25" t="n">
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
@@ -2132,7 +2136,7 @@
       <c r="K22" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="L22" s="20" t="n">
+      <c r="L22" s="21" t="n">
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
@@ -2167,7 +2171,7 @@
       <c r="K23" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="L23" s="23" t="n">
+      <c r="L23" s="24" t="n">
         <f aca="false">$N$11</f>
         <v>123456789</v>
       </c>
@@ -2501,8 +2505,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N20:Q20"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2524,7 +2529,7 @@
   <dimension ref="C13:J36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="O21:Q25 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>